<commit_message>
removed problematic shortened ... char that gets mangled by some programs when converting to csv
</commit_message>
<xml_diff>
--- a/DatasetTemplate/samples.xlsx
+++ b/DatasetTemplate/samples.xlsx
@@ -41,7 +41,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>MINDS Fields…</t>
+    <t>MINDS Fields</t>
   </si>
   <si>
     <t>specimen</t>
@@ -50,7 +50,7 @@
     <t>specimen anatomical location</t>
   </si>
   <si>
-    <t>Additional Fields (e.g. MINDS)…</t>
+    <t>Additional Fields (e.g. MINDS)</t>
   </si>
   <si>
     <t>species</t>

</xml_diff>